<commit_message>
modified Searchv4 test data file
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData_V4.xlsx
+++ b/src/test/test-data/SearchTestData_V4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12825" windowHeight="6810"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="362">
   <si>
     <t>API</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>?query=HIV Wom?n&amp;size=1</t>
-  </si>
-  <si>
-    <t>?query=wo?&amp;size=1</t>
   </si>
   <si>
     <t>?query=food wo*&amp;size=1</t>
@@ -883,9 +880,6 @@
     <t>/wos/details/(OPQA-734_hits.id)</t>
   </si>
   <si>
-    <t>/wos/details/(OPQA-254_hits.id)</t>
-  </si>
-  <si>
     <t>/wos/details/(OPQA-252_hits.id)</t>
   </si>
   <si>
@@ -1105,6 +1099,18 @@
   </si>
   <si>
     <t>status=200||hits.fields."snid"=0028-0836</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>hits.id[0]</t>
+  </si>
+  <si>
+    <t>/wos/details/(OPQA-254_hits.id[0])</t>
+  </si>
+  <si>
+    <t>?query=bi?&amp;size=10</t>
   </si>
 </sst>
 </file>
@@ -1544,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1604,42 +1610,45 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
         <v>240</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>242</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="J2" t="s">
-        <v>267</v>
-      </c>
       <c r="K2" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="L2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -1657,18 +1666,21 @@
         <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -1678,26 +1690,29 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K4" s="1"/>
+      <c r="L4" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -1707,29 +1722,32 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K5" s="1"/>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
@@ -1738,22 +1756,25 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K6" s="1"/>
+      <c r="L6" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -1771,16 +1792,19 @@
         <v>14</v>
       </c>
       <c r="K7" s="1"/>
+      <c r="L7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -1798,16 +1822,19 @@
         <v>14</v>
       </c>
       <c r="K8" s="1"/>
+      <c r="L8" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -1825,16 +1852,19 @@
         <v>14</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -1852,16 +1882,19 @@
         <v>14</v>
       </c>
       <c r="K10" s="1"/>
+      <c r="L10" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -1879,16 +1912,19 @@
         <v>14</v>
       </c>
       <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -1906,16 +1942,19 @@
         <v>14</v>
       </c>
       <c r="K12" s="1"/>
+      <c r="L12" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -1933,16 +1972,19 @@
         <v>14</v>
       </c>
       <c r="K13" s="1"/>
+      <c r="L13" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -1960,16 +2002,19 @@
         <v>14</v>
       </c>
       <c r="K14" s="1"/>
+      <c r="L14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -1987,16 +2032,19 @@
         <v>14</v>
       </c>
       <c r="K15" s="1"/>
+      <c r="L15" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -2006,7 +2054,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2014,16 +2062,19 @@
         <v>14</v>
       </c>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -2041,16 +2092,19 @@
         <v>14</v>
       </c>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" ht="30">
+      <c r="L17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -2060,7 +2114,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2068,16 +2122,19 @@
         <v>14</v>
       </c>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
@@ -2087,7 +2144,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2095,163 +2152,184 @@
         <v>14</v>
       </c>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+      <c r="L19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H20"/>
       <c r="J20" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="180">
+        <v>281</v>
+      </c>
+      <c r="L20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="180">
       <c r="A21" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="180">
+        <v>292</v>
+      </c>
+      <c r="L21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="180">
       <c r="A22" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J22" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="L22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="180">
+      <c r="A23" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="180">
-      <c r="A23" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="180">
+        <v>292</v>
+      </c>
+      <c r="L23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="180">
       <c r="A24" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="180">
+        <v>292</v>
+      </c>
+      <c r="L24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="180">
       <c r="A25" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>292</v>
+      </c>
+      <c r="L25" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
@@ -2267,42 +2345,48 @@
         <v>14</v>
       </c>
       <c r="K26" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="75">
+        <v>280</v>
+      </c>
+      <c r="L26" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="75">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="H27"/>
       <c r="I27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+        <v>289</v>
+      </c>
+      <c r="L27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>12</v>
@@ -2311,49 +2395,52 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>28</v>
+        <v>361</v>
       </c>
       <c r="H28"/>
       <c r="J28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="75">
+        <v>359</v>
+      </c>
+      <c r="L28" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="75">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>286</v>
+        <v>360</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
       </c>
       <c r="H29"/>
       <c r="I29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>12</v>
@@ -2362,38 +2449,44 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H30"/>
       <c r="J30" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K30" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="135">
+        <v>280</v>
+      </c>
+      <c r="L30" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="135">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
       </c>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="L31" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2406,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L34"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2462,23 +2555,23 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
@@ -2486,46 +2579,52 @@
         <v>14</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
+      </c>
+      <c r="L2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G3"/>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K3"/>
+      <c r="L3" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>1</v>
@@ -2534,63 +2633,69 @@
       <c r="G4" s="10"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="L4" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="K5" s="10"/>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="1"/>
@@ -2598,55 +2703,61 @@
         <v>14</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c r="L6" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="60">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K7"/>
+      <c r="L7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2654,26 +2765,29 @@
         <v>14</v>
       </c>
       <c r="K8" s="1"/>
+      <c r="L8" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2681,459 +2795,516 @@
         <v>14</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K10"/>
+      <c r="L10" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K11"/>
+      <c r="L11" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>215</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
+      </c>
+      <c r="L12" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>218</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K13" s="5"/>
+      <c r="L13" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K14" s="5"/>
+      <c r="L14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>222</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K15" s="5"/>
+      <c r="L15" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>224</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>227</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>230</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="30">
+      <c r="L18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45">
+      <c r="A20" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" ht="45">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30">
+      <c r="A21" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>238</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+      <c r="L21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="270">
+        <v>281</v>
+      </c>
+      <c r="L22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="270">
       <c r="A23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="G23"/>
       <c r="I23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11" ht="270">
+      <c r="L23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="270">
       <c r="A24" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="G24"/>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K24"/>
-    </row>
-    <row r="25" spans="1:11" ht="270">
+      <c r="L24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="270">
       <c r="A25" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="G25"/>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K25"/>
-    </row>
-    <row r="26" spans="1:11" ht="270">
+      <c r="L25" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="270">
       <c r="A26" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="G26"/>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K26"/>
-    </row>
-    <row r="27" spans="1:11" ht="270">
+      <c r="L26" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="270">
       <c r="A27" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="G27"/>
       <c r="I27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K27"/>
+      <c r="L27" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3151,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="L22" sqref="L2:L22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3211,13 +3382,13 @@
     </row>
     <row r="2" spans="1:12" s="16" customFormat="1" ht="30">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -3227,35 +3398,37 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="L2"/>
+      <c r="L2" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
@@ -3263,21 +3436,24 @@
         <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -3290,19 +3466,22 @@
         <v>14</v>
       </c>
       <c r="K4" s="1"/>
+      <c r="L4" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1</v>
@@ -3311,63 +3490,69 @@
       <c r="G5" s="10"/>
       <c r="H5" s="8"/>
       <c r="I5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="L5" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="K6" s="10"/>
+      <c r="L6" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="1"/>
@@ -3375,57 +3560,63 @@
         <v>14</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c r="L7" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K8" s="1"/>
+      <c r="L8" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -3433,26 +3624,29 @@
         <v>14</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -3460,26 +3654,29 @@
         <v>14</v>
       </c>
       <c r="K10" s="1"/>
+      <c r="L10" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -3487,26 +3684,29 @@
         <v>14</v>
       </c>
       <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -3514,26 +3714,29 @@
         <v>14</v>
       </c>
       <c r="K12" s="1"/>
+      <c r="L12" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="1"/>
@@ -3541,86 +3744,95 @@
         <v>14</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="L13" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>203</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K14" s="1"/>
+      <c r="L14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>205</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K15" s="1"/>
+      <c r="L15" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="1"/>
@@ -3628,93 +3840,105 @@
         <v>14</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30">
+        <v>326</v>
+      </c>
+      <c r="L16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>209</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" ht="30">
+      <c r="L17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30">
       <c r="A18" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" ht="30">
+      <c r="L18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75">
+      <c r="L19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="8"/>
       <c r="B20" s="13"/>
       <c r="C20" s="9"/>
@@ -3722,7 +3946,7 @@
       <c r="H20"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="8"/>
       <c r="B21" s="13"/>
       <c r="C21" s="9"/>
@@ -3731,7 +3955,7 @@
       <c r="H21" s="11"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75">
+    <row r="22" spans="1:12" ht="15.75">
       <c r="A22" s="8"/>
       <c r="B22" s="13"/>
       <c r="C22" s="9"/>
@@ -3811,23 +4035,23 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
@@ -3835,71 +4059,80 @@
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="G3"/>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
+      </c>
+      <c r="L3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>106</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L4" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" t="s">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
-        <v>109</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -3908,51 +4141,57 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
       <c r="I5" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K5" s="1"/>
+      <c r="L5" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="31.5">
       <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>112</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L6" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
@@ -3961,51 +4200,57 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
       <c r="I7" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K7" s="1"/>
+      <c r="L7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>117</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>118</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L8" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
@@ -4014,196 +4259,220 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
       <c r="I9" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>123</v>
-      </c>
       <c r="J10" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="L10" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75">
       <c r="A11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>126</v>
-      </c>
       <c r="J11" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="31.5">
       <c r="A12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C12" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>129</v>
-      </c>
       <c r="J12" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K12" s="1"/>
+      <c r="L12" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>132</v>
-      </c>
       <c r="J13" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K13" s="1"/>
+      <c r="L13" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>134</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>135</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="L14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="31.5">
       <c r="A15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>137</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>138</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="L15" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -4211,6 +4480,9 @@
         <v>14</v>
       </c>
       <c r="K17" s="8"/>
+      <c r="L17" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4222,8 +4494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4282,13 +4554,13 @@
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>154</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -4298,80 +4570,89 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K2" s="1"/>
+      <c r="L2" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="L3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
       <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>160</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J4" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="L4" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>1</v>
@@ -4380,119 +4661,131 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="L5" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K6" s="10"/>
+      <c r="L6" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c r="L7" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
+      </c>
+      <c r="L8" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="1"/>
@@ -4500,67 +4793,76 @@
         <v>14</v>
       </c>
       <c r="K9" s="1"/>
+      <c r="L9" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="H10"/>
       <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L10" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L11" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>248</v>
-      </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -4573,145 +4875,163 @@
         <v>14</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
+      </c>
+      <c r="L12" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
+      </c>
+      <c r="L13" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
+      </c>
+      <c r="L14" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="31.5">
       <c r="A15" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>256</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>257</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J15" t="s">
-        <v>348</v>
+        <v>346</v>
+      </c>
+      <c r="L15" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="31.5">
       <c r="A16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>260</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>261</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>347</v>
+      </c>
+      <c r="L16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
+        <v>261</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>265</v>
-      </c>
       <c r="F17" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K17" s="8"/>
+      <c r="L17" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified Searchv4 test data
</commit_message>
<xml_diff>
--- a/src/test/test-data/SearchTestData_V4.xlsx
+++ b/src/test/test-data/SearchTestData_V4.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="362">
   <si>
     <t>API</t>
   </si>
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1636,9 +1636,6 @@
       <c r="K2" t="s">
         <v>245</v>
       </c>
-      <c r="L2" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
@@ -1668,9 +1665,6 @@
       <c r="K3" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="L3" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
@@ -1700,9 +1694,6 @@
         <v>287</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
@@ -1732,9 +1723,6 @@
         <v>287</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
@@ -1762,9 +1750,6 @@
         <v>287</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
@@ -1792,9 +1777,6 @@
         <v>14</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
@@ -1822,9 +1804,6 @@
         <v>14</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="1" t="s">
@@ -1852,9 +1831,6 @@
         <v>14</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="1" t="s">
@@ -1882,9 +1858,6 @@
         <v>14</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
@@ -1912,9 +1885,6 @@
         <v>14</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
@@ -1942,9 +1912,6 @@
         <v>14</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="1" t="s">
@@ -1972,9 +1939,6 @@
         <v>14</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
@@ -2002,9 +1966,6 @@
         <v>14</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
@@ -2032,9 +1993,6 @@
         <v>14</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="1" t="s">
@@ -2062,11 +2020,8 @@
         <v>14</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -2092,11 +2047,8 @@
         <v>14</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30">
+    </row>
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -2122,11 +2074,8 @@
         <v>14</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
@@ -2152,11 +2101,8 @@
         <v>14</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45">
+    </row>
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -2182,11 +2128,8 @@
       <c r="K20" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="L20" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="180">
+    </row>
+    <row r="21" spans="1:11" ht="180">
       <c r="A21" s="1" t="s">
         <v>273</v>
       </c>
@@ -2209,11 +2152,8 @@
       <c r="J21" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="L21" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="180">
+    </row>
+    <row r="22" spans="1:11" ht="180">
       <c r="A22" s="1" t="s">
         <v>274</v>
       </c>
@@ -2236,11 +2176,8 @@
       <c r="J22" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="L22" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="180">
+    </row>
+    <row r="23" spans="1:11" ht="180">
       <c r="A23" s="1" t="s">
         <v>275</v>
       </c>
@@ -2263,11 +2200,8 @@
       <c r="J23" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="L23" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="180">
+    </row>
+    <row r="24" spans="1:11" ht="180">
       <c r="A24" s="1" t="s">
         <v>276</v>
       </c>
@@ -2290,11 +2224,8 @@
       <c r="J24" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="L24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="180">
+    </row>
+    <row r="25" spans="1:11" ht="180">
       <c r="A25" s="1" t="s">
         <v>277</v>
       </c>
@@ -2317,11 +2248,8 @@
       <c r="J25" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="L25" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -2347,11 +2275,8 @@
       <c r="K26" t="s">
         <v>280</v>
       </c>
-      <c r="L26" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="75">
+    </row>
+    <row r="27" spans="1:11" ht="75">
       <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
@@ -2374,11 +2299,8 @@
       <c r="J27" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="L27" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="30">
+    </row>
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
@@ -2404,11 +2326,8 @@
       <c r="K28" t="s">
         <v>359</v>
       </c>
-      <c r="L28" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="75">
+    </row>
+    <row r="29" spans="1:11" ht="75">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -2432,7 +2351,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30">
+    <row r="30" spans="1:11" ht="30">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -2458,11 +2377,8 @@
       <c r="K30" t="s">
         <v>280</v>
       </c>
-      <c r="L30" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="135">
+    </row>
+    <row r="31" spans="1:11" ht="135">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
@@ -2484,9 +2400,6 @@
       </c>
       <c r="J31" s="7" t="s">
         <v>291</v>
-      </c>
-      <c r="L31" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>